<commit_message>
Resolved blanked value being too high. Added calibration files.
</commit_message>
<xml_diff>
--- a/Calibration/Calibration_Curve.xlsx
+++ b/Calibration/Calibration_Curve.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felixekness/Documents/Academic/Graduate School/Semesters/Fall '15/BIOE 521/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felixekness/Documents/Academic/Graduate School/Semesters/Fall '15/BIOE 521/code/Team04_MicrobeControllers/Calibration/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="4900" yWindow="840" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>blank</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>Spec Readings (OD) 11/17/2015</t>
+  </si>
+  <si>
+    <t>Raw OD</t>
+  </si>
+  <si>
+    <t>Mapped OD</t>
   </si>
 </sst>
 </file>
@@ -100,25 +106,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,8 +405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -408,131 +415,131 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="5"/>
-      <c r="N1" s="2" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="7"/>
+      <c r="N1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
     </row>
     <row r="2" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="2">
         <v>0.05</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="2">
         <v>0.1</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="2">
         <v>0.15</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="2">
         <v>0.2</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="2">
         <v>0.21</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="2">
         <v>0.25</v>
       </c>
-      <c r="J2" s="6">
+      <c r="J2" s="2">
         <v>0.3</v>
       </c>
-      <c r="K2" s="6">
+      <c r="K2" s="2">
         <v>0.5</v>
       </c>
-      <c r="L2" s="7">
+      <c r="L2" s="3">
         <v>1</v>
       </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="O2" s="6">
+      <c r="O2" s="2">
         <v>0.05</v>
       </c>
-      <c r="P2" s="6">
+      <c r="P2" s="2">
         <v>0.1</v>
       </c>
-      <c r="Q2" s="6">
+      <c r="Q2" s="2">
         <v>0.15</v>
       </c>
-      <c r="R2" s="6">
+      <c r="R2" s="2">
         <v>0.2</v>
       </c>
-      <c r="S2" s="6">
+      <c r="S2" s="2">
         <v>0.21</v>
       </c>
-      <c r="T2" s="6">
+      <c r="T2" s="2">
         <v>0.25</v>
       </c>
-      <c r="U2" s="6">
+      <c r="U2" s="2">
         <v>0.3</v>
       </c>
-      <c r="V2" s="6">
+      <c r="V2" s="2">
         <v>0.5</v>
       </c>
-      <c r="W2" s="6">
+      <c r="W2" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B3" s="8">
+      <c r="B3" s="4">
         <v>5348</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="4">
         <v>10352</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="4">
         <v>9419</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="4">
         <v>8698</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="4">
         <v>7327</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="4">
         <v>6918</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="4">
         <v>6839</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="4">
         <v>6400</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="4">
         <v>6185</v>
       </c>
-      <c r="K3" s="8">
+      <c r="K3" s="4">
         <v>4418</v>
       </c>
-      <c r="L3" s="9">
+      <c r="L3" s="5">
         <v>1867</v>
       </c>
       <c r="M3" s="1" t="s">
@@ -543,41 +550,41 @@
       </c>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B4" s="8">
+      <c r="B4" s="4">
         <v>5356</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="4">
         <v>10354</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="4">
         <v>9420</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="4">
         <v>8707</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="4">
         <v>7347</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="4">
         <v>6919</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="4">
         <v>6838</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="4">
         <v>6403</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4" s="4">
         <v>6163</v>
       </c>
-      <c r="K4" s="8">
+      <c r="K4" s="4">
         <v>4422</v>
       </c>
-      <c r="L4" s="9">
+      <c r="L4" s="5">
         <v>1866</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -611,492 +618,525 @@
       </c>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B5" s="8">
+      <c r="B5" s="4">
         <v>5385</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="4">
         <v>10352</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="4">
         <v>9419</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="4">
         <v>8712</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="4">
         <v>7321</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="4">
         <v>6906</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="4">
         <v>6837</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="4">
         <v>6404</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5" s="4">
         <v>6164</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K5" s="4">
         <v>4423</v>
       </c>
-      <c r="L5" s="9">
+      <c r="L5" s="5">
         <v>1866</v>
       </c>
+      <c r="M5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N5" s="10">
+        <v>0</v>
+      </c>
+      <c r="O5" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="P5" s="10">
+        <v>0.09</v>
+      </c>
+      <c r="Q5" s="10">
+        <v>0.13</v>
+      </c>
+      <c r="R5" s="10">
+        <v>0.16</v>
+      </c>
+      <c r="S5" s="10">
+        <v>0.18</v>
+      </c>
+      <c r="T5" s="10">
+        <v>0.21</v>
+      </c>
+      <c r="U5" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="V5" s="10">
+        <v>0.41</v>
+      </c>
+      <c r="W5" s="10">
+        <v>0.94</v>
+      </c>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B6" s="8">
+      <c r="B6" s="4">
         <v>5386</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="4">
         <v>10350</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="4">
         <v>9419</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="4">
         <v>8716</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="4">
         <v>7324</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="4">
         <v>6904</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="4">
         <v>6836</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="4">
         <v>6405</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J6" s="4">
         <v>6165</v>
       </c>
-      <c r="K6" s="8">
+      <c r="K6" s="4">
         <v>4424</v>
       </c>
-      <c r="L6" s="9">
+      <c r="L6" s="5">
         <v>1867</v>
       </c>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B7" s="8">
+      <c r="B7" s="4">
         <v>5386</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="4">
         <v>10348</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="4">
         <v>9419</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="4">
         <v>8715</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="4">
         <v>7369</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="4">
         <v>6901</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="4">
         <v>6834</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="4">
         <v>6407</v>
       </c>
-      <c r="J7" s="8">
+      <c r="J7" s="4">
         <v>6163</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K7" s="4">
         <v>4423</v>
       </c>
-      <c r="L7" s="9">
+      <c r="L7" s="5">
         <v>1867</v>
       </c>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B8" s="8">
+      <c r="B8" s="4">
         <v>5387</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="4">
         <v>10353</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="4">
         <v>9421</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="4">
         <v>8715</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="4">
         <v>7377</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="4">
         <v>6902</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="4">
         <v>6832</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="4">
         <v>6407</v>
       </c>
-      <c r="J8" s="8">
+      <c r="J8" s="4">
         <v>6162</v>
       </c>
-      <c r="K8" s="8">
+      <c r="K8" s="4">
         <v>4440</v>
       </c>
-      <c r="L8" s="9">
+      <c r="L8" s="5">
         <v>1868</v>
       </c>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B9" s="8">
+      <c r="B9" s="4">
         <v>5383</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="4">
         <v>10348</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="4">
         <v>9424</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="4">
         <v>8722</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="4">
         <v>7375</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="4">
         <v>6901</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="4">
         <v>6831</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="4">
         <v>6396</v>
       </c>
-      <c r="J9" s="8">
+      <c r="J9" s="4">
         <v>6173</v>
       </c>
-      <c r="K9" s="8">
+      <c r="K9" s="4">
         <v>4433</v>
       </c>
-      <c r="L9" s="9">
+      <c r="L9" s="5">
         <v>1868</v>
       </c>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B10" s="8">
+      <c r="B10" s="4">
         <v>5338</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="4">
         <v>10343</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="4">
         <v>9426</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="4">
         <v>8722</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="4">
         <v>7369</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="4">
         <v>6902</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="4">
         <v>6831</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I10" s="4">
         <v>6388</v>
       </c>
-      <c r="J10" s="8">
+      <c r="J10" s="4">
         <v>6186</v>
       </c>
-      <c r="K10" s="8">
+      <c r="K10" s="4">
         <v>4421</v>
       </c>
-      <c r="L10" s="9">
+      <c r="L10" s="5">
         <v>1868</v>
       </c>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B11" s="8">
+      <c r="B11" s="4">
         <v>5331</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="4">
         <v>10343</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="4">
         <v>9428</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="4">
         <v>8739</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="4">
         <v>7364</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="4">
         <v>6899</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="4">
         <v>6832</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I11" s="4">
         <v>6370</v>
       </c>
-      <c r="J11" s="8">
+      <c r="J11" s="4">
         <v>6186</v>
       </c>
-      <c r="K11" s="8">
+      <c r="K11" s="4">
         <v>4419</v>
       </c>
-      <c r="L11" s="9">
+      <c r="L11" s="5">
         <v>1868</v>
       </c>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B12" s="8">
+      <c r="B12" s="4">
         <v>5326</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="4">
         <v>10343</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="4">
         <v>9431</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="4">
         <v>8744</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="4">
         <v>7372</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="4">
         <v>6900</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="4">
         <v>6834</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="4">
         <v>6373</v>
       </c>
-      <c r="J12" s="8">
+      <c r="J12" s="4">
         <v>6187</v>
       </c>
-      <c r="K12" s="8">
+      <c r="K12" s="4">
         <v>4429</v>
       </c>
-      <c r="L12" s="9">
+      <c r="L12" s="5">
         <v>1869</v>
       </c>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B13" s="8">
+      <c r="B13" s="4">
         <v>5326</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="4">
         <v>10341</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="4">
         <v>9429</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="4">
         <v>8738</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="4">
         <v>7375</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="4">
         <v>6899</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="4">
         <v>6804</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="4">
         <v>6372</v>
       </c>
-      <c r="J13" s="8">
+      <c r="J13" s="4">
         <v>6186</v>
       </c>
-      <c r="K13" s="8">
+      <c r="K13" s="4">
         <v>4441</v>
       </c>
-      <c r="L13" s="9">
+      <c r="L13" s="5">
         <v>1870</v>
       </c>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B14" s="8">
+      <c r="B14" s="4">
         <v>5325</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="4">
         <v>10341</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="4">
         <v>9427</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="4">
         <v>8739</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="4">
         <v>7375</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="4">
         <v>6896</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="4">
         <v>6804</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14" s="4">
         <v>6372</v>
       </c>
-      <c r="J14" s="8">
+      <c r="J14" s="4">
         <v>6183</v>
       </c>
-      <c r="K14" s="8">
+      <c r="K14" s="4">
         <v>4441</v>
       </c>
-      <c r="L14" s="9">
+      <c r="L14" s="5">
         <v>1868</v>
       </c>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B15" s="8">
+      <c r="B15" s="4">
         <v>5373</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="4">
         <v>10340</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="4">
         <v>9426</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="4">
         <v>8740</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="4">
         <v>7375</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="4">
         <v>6894</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H15" s="4">
         <v>6800</v>
       </c>
-      <c r="I15" s="8">
+      <c r="I15" s="4">
         <v>6372</v>
       </c>
-      <c r="J15" s="8">
+      <c r="J15" s="4">
         <v>6181</v>
       </c>
-      <c r="K15" s="8">
+      <c r="K15" s="4">
         <v>4441</v>
       </c>
-      <c r="L15" s="9">
+      <c r="L15" s="5">
         <v>1868</v>
       </c>
     </row>
     <row r="16" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B16" s="8">
+      <c r="B16" s="4">
         <v>5358</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="4">
         <v>10340</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="4">
         <v>9423</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="4">
         <v>8739</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="4">
         <v>7374</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="4">
         <v>6893</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H16" s="4">
         <v>6800</v>
       </c>
-      <c r="I16" s="8">
+      <c r="I16" s="4">
         <v>6374</v>
       </c>
-      <c r="J16" s="8">
+      <c r="J16" s="4">
         <v>6178</v>
       </c>
-      <c r="K16" s="8">
+      <c r="K16" s="4">
         <v>4442</v>
       </c>
-      <c r="L16" s="9">
+      <c r="L16" s="5">
         <v>1868</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="B17" s="8">
+      <c r="B17" s="4">
         <v>5361</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="4">
         <v>10340</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="4">
         <v>9418</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="4">
         <v>8691</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="4">
         <v>7374</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="4">
         <v>6881</v>
       </c>
-      <c r="H17" s="8">
+      <c r="H17" s="4">
         <v>6799</v>
       </c>
-      <c r="I17" s="8">
+      <c r="I17" s="4">
         <v>6376</v>
       </c>
-      <c r="J17" s="8">
+      <c r="J17" s="4">
         <v>6177</v>
       </c>
-      <c r="K17" s="8">
+      <c r="K17" s="4">
         <v>4427</v>
       </c>
-      <c r="L17" s="9">
+      <c r="L17" s="5">
         <v>1872</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="B18" s="8">
+      <c r="B18" s="4">
         <v>5361</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="4">
         <v>10338</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="4">
         <v>9415</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="4">
         <v>8690</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F18" s="4">
         <v>7374</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="4">
         <v>6890</v>
       </c>
-      <c r="H18" s="8">
+      <c r="H18" s="4">
         <v>6795</v>
       </c>
-      <c r="I18" s="8">
+      <c r="I18" s="4">
         <v>6376</v>
       </c>
-      <c r="J18" s="8">
+      <c r="J18" s="4">
         <v>6161</v>
       </c>
-      <c r="K18" s="8">
+      <c r="K18" s="4">
         <v>4427</v>
       </c>
-      <c r="L18" s="9">
+      <c r="L18" s="5">
         <v>1872</v>
       </c>
     </row>
@@ -1104,47 +1144,47 @@
       <c r="A19" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="4">
         <f t="shared" ref="B19:L19" si="0">AVERAGE(B3:B18)</f>
         <v>5358.125</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="4">
         <f t="shared" si="0"/>
         <v>10345.375</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D19" s="4">
         <f t="shared" si="0"/>
         <v>9422.75</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="4">
         <f t="shared" si="0"/>
         <v>8720.4375</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F19" s="4">
         <f t="shared" si="0"/>
         <v>7362</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="4">
         <f t="shared" si="0"/>
         <v>6900.3125</v>
       </c>
-      <c r="H19" s="8">
+      <c r="H19" s="4">
         <f t="shared" si="0"/>
         <v>6821.625</v>
       </c>
-      <c r="I19" s="8">
+      <c r="I19" s="4">
         <f t="shared" si="0"/>
         <v>6387.1875</v>
       </c>
-      <c r="J19" s="8">
+      <c r="J19" s="4">
         <f t="shared" si="0"/>
         <v>6175</v>
       </c>
-      <c r="K19" s="8">
+      <c r="K19" s="4">
         <f t="shared" si="0"/>
         <v>4429.4375</v>
       </c>
-      <c r="L19" s="9">
+      <c r="L19" s="5">
         <f t="shared" si="0"/>
         <v>1868.25</v>
       </c>
@@ -1153,93 +1193,93 @@
       <c r="A20" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8">
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4">
         <f>-LOG10(D19/C19)</f>
         <v>4.0568568856252242E-2</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="4">
         <f>-LOG10(E19/C19)</f>
         <v>7.420796381232149E-2</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F20" s="4">
         <f>-LOG10(F19/C19)</f>
         <v>0.14775042451836395</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="4">
         <f>-LOG10(G19/C19)</f>
         <v>0.17587747820300506</v>
       </c>
-      <c r="H20" s="8">
+      <c r="H20" s="4">
         <f>-LOG10(H19/C19)</f>
         <v>0.18085839604151396</v>
       </c>
-      <c r="I20" s="8">
+      <c r="I20" s="4">
         <f>-LOG10(I19/C19)</f>
         <v>0.20943657228985776</v>
       </c>
-      <c r="J20" s="8">
+      <c r="J20" s="4">
         <f>-LOG10(J19/C19)</f>
         <v>0.22410927569730851</v>
       </c>
-      <c r="K20" s="8">
+      <c r="K20" s="4">
         <f>-LOG10(K19/C19)</f>
         <v>0.36839765952260295</v>
       </c>
-      <c r="L20" s="9">
+      <c r="L20" s="5">
         <f>-LOG10(L19/C19)</f>
         <v>0.74331124670080528</v>
       </c>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
-      <c r="T20" s="3"/>
-      <c r="U20" s="3"/>
-      <c r="V20" s="3"/>
-      <c r="W20" s="3"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="9"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="D25" s="6">
+      <c r="D25" s="2">
         <v>0.05</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="2">
         <v>0.1</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25" s="2">
         <v>0.15</v>
       </c>
-      <c r="G25" s="6">
+      <c r="G25" s="2">
         <v>0.2</v>
       </c>
-      <c r="H25" s="6">
+      <c r="H25" s="2">
         <v>0.21</v>
       </c>
-      <c r="I25" s="6">
+      <c r="I25" s="2">
         <v>0.25</v>
       </c>
-      <c r="J25" s="6">
+      <c r="J25" s="2">
         <v>0.3</v>
       </c>
-      <c r="K25" s="6">
+      <c r="K25" s="2">
         <v>0.5</v>
       </c>
-      <c r="L25" s="6">
+      <c r="L25" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>